<commit_message>
Rajout de la partie d'Anis sur la DCT
</commit_message>
<xml_diff>
--- a/Rapport/2-approcheCommerciale/MIG Eco Excel.xlsx
+++ b/Rapport/2-approcheCommerciale/MIG Eco Excel.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="61">
   <si>
     <t>Ce document a été exporté depuis Numbers. Chaque tableau a été converti en feuille de calcul Excel. Tous les autres objets sur chaque feuille Numbers ont été placés sur des feuilles de calcul différentes. Veuillez noter que les calculs de formules peuvent être différents dans Excel.</t>
   </si>
@@ -128,6 +128,9 @@
   </si>
   <si>
     <t>Licences</t>
+  </si>
+  <si>
+    <t>2 serveurs</t>
   </si>
   <si>
     <t>Impots</t>
@@ -483,7 +486,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -568,9 +571,6 @@
     </xf>
     <xf numFmtId="59" fontId="6" fillId="6" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
@@ -738,7 +738,7 @@
     </row>
     <row r="13">
       <c r="B13" t="s" s="3">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -746,15 +746,15 @@
     <row r="14">
       <c r="B14" s="4"/>
       <c r="C14" t="s" s="4">
+        <v>39</v>
+      </c>
+      <c r="D14" t="s" s="5">
         <v>38</v>
-      </c>
-      <c r="D14" t="s" s="5">
-        <v>37</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" t="s" s="3">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -762,19 +762,19 @@
     <row r="16">
       <c r="B16" s="4"/>
       <c r="C16" t="s" s="4">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D16" t="s" s="5">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" s="4"/>
       <c r="C17" t="s" s="4">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D17" t="s" s="5">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1148,23 +1148,23 @@
         <v>25</v>
       </c>
       <c r="C17" s="11">
-        <v>2750</v>
+        <v>2700</v>
       </c>
       <c r="D17" s="11">
         <f>C17*0.22</f>
-        <v>605</v>
+        <v>594</v>
       </c>
       <c r="E17" s="11">
         <f>C17-D17</f>
-        <v>2145</v>
+        <v>2106</v>
       </c>
       <c r="F17" s="11">
         <f>C17*0.44</f>
-        <v>1210</v>
+        <v>1188</v>
       </c>
       <c r="G17" s="12">
         <f>C17+F17</f>
-        <v>3960</v>
+        <v>3888</v>
       </c>
     </row>
     <row r="18" ht="24" customHeight="1">
@@ -1173,23 +1173,23 @@
       </c>
       <c r="C18" s="15">
         <f>SUM(C4:C17)</f>
-        <v>30690</v>
+        <v>30640</v>
       </c>
       <c r="D18" s="15">
         <f>SUM(D4:D17)</f>
-        <v>6751.800000000001</v>
+        <v>6740.800000000001</v>
       </c>
       <c r="E18" s="15">
         <f>SUM(E4:E17)</f>
-        <v>23938.2</v>
+        <v>23899.2</v>
       </c>
       <c r="F18" s="15">
         <f>SUM(F4:F17)</f>
-        <v>13503.6</v>
+        <v>13481.6</v>
       </c>
       <c r="G18" s="15">
         <f>SUM(G4:G17)</f>
-        <v>44193.599999999991</v>
+        <v>44121.599999999991</v>
       </c>
     </row>
   </sheetData>
@@ -1276,7 +1276,8 @@
         <v>4</v>
       </c>
       <c r="I3" s="26">
-        <v>45777</v>
+        <f>'Salaires - Salaires'!G18</f>
+        <v>44121.599999999991</v>
       </c>
     </row>
     <row r="4" ht="23" customHeight="1">
@@ -1292,18 +1293,18 @@
         <v>5.004</v>
       </c>
       <c r="F4" s="29">
-        <v>24000</v>
+        <v>26000</v>
       </c>
       <c r="G4" s="26">
         <f>E4*F4</f>
-        <v>120096</v>
+        <v>130104</v>
       </c>
       <c r="H4" t="s" s="25">
         <v>35</v>
       </c>
       <c r="I4" s="26">
         <f>F4</f>
-        <v>24000</v>
+        <v>26000</v>
       </c>
     </row>
     <row r="5" ht="24" customHeight="1">
@@ -1325,23 +1326,28 @@
         <f>E5*F5</f>
         <v>9999.995999999999</v>
       </c>
-      <c r="H5" s="31"/>
-      <c r="I5" s="26"/>
+      <c r="H5" t="s" s="25">
+        <v>37</v>
+      </c>
+      <c r="I5" s="26">
+        <f>12*606</f>
+        <v>7272</v>
+      </c>
     </row>
     <row r="6" ht="24" customHeight="1">
-      <c r="B6" t="s" s="32">
+      <c r="B6" t="s" s="31">
         <v>26</v>
       </c>
-      <c r="C6" s="33">
+      <c r="C6" s="32">
         <f>SUM(G3:G5)-SUM(I3:I5)</f>
-        <v>60318.995999999985</v>
-      </c>
-      <c r="D6" s="34"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34"/>
-      <c r="I6" s="36"/>
+        <v>62710.395999999993</v>
+      </c>
+      <c r="D6" s="33"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1371,43 +1377,43 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.25" defaultRowHeight="21" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="0.25" style="37" customWidth="1"/>
-    <col min="2" max="2" width="12.25" style="37" customWidth="1"/>
-    <col min="3" max="3" width="12.25" style="37" customWidth="1"/>
-    <col min="4" max="4" width="12.25" style="37" customWidth="1"/>
-    <col min="5" max="256" width="12.25" style="37" customWidth="1"/>
+    <col min="1" max="1" width="0.25" style="36" customWidth="1"/>
+    <col min="2" max="2" width="12.25" style="36" customWidth="1"/>
+    <col min="3" max="3" width="12.25" style="36" customWidth="1"/>
+    <col min="4" max="4" width="12.25" style="36" customWidth="1"/>
+    <col min="5" max="256" width="12.25" style="36" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="2" customHeight="1"/>
     <row r="2" ht="22" customHeight="1">
-      <c r="B2" t="s" s="38">
-        <v>39</v>
-      </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="40"/>
+      <c r="B2" t="s" s="37">
+        <v>40</v>
+      </c>
+      <c r="C2" s="38"/>
+      <c r="D2" s="39"/>
     </row>
     <row r="3" ht="22" customHeight="1">
-      <c r="B3" t="s" s="41">
-        <v>40</v>
-      </c>
-      <c r="C3" t="s" s="42">
+      <c r="B3" t="s" s="40">
         <v>41</v>
       </c>
-      <c r="D3" s="43">
+      <c r="C3" t="s" s="41">
+        <v>42</v>
+      </c>
+      <c r="D3" s="42">
         <f>0.33*'Bilan - Tableau 2'!B1</f>
-        <v>11318.932944</v>
+        <v>11447.566944</v>
       </c>
     </row>
     <row r="4" ht="22" customHeight="1">
-      <c r="B4" t="s" s="41">
-        <v>42</v>
-      </c>
-      <c r="C4" t="s" s="44">
+      <c r="B4" t="s" s="40">
         <v>43</v>
       </c>
-      <c r="D4" s="45">
+      <c r="C4" t="s" s="43">
+        <v>44</v>
+      </c>
+      <c r="D4" s="44">
         <f>0.2*'Compte de résultat prévisionnel'!G4+0.2*'Compte de résultat prévisionnel'!G5</f>
-        <v>26019.1992</v>
+        <v>28020.7992</v>
       </c>
     </row>
   </sheetData>
@@ -1435,85 +1441,85 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.25" defaultRowHeight="21" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="14.3125" style="46" customWidth="1"/>
-    <col min="2" max="2" width="12.25" style="46" customWidth="1"/>
-    <col min="3" max="3" width="12.25" style="46" customWidth="1"/>
-    <col min="4" max="4" width="12.25" style="46" customWidth="1"/>
-    <col min="5" max="256" width="12.25" style="46" customWidth="1"/>
+    <col min="1" max="1" width="14.3125" style="45" customWidth="1"/>
+    <col min="2" max="2" width="12.25" style="45" customWidth="1"/>
+    <col min="3" max="3" width="12.25" style="45" customWidth="1"/>
+    <col min="4" max="4" width="12.25" style="45" customWidth="1"/>
+    <col min="5" max="256" width="12.25" style="45" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="23" customHeight="1">
-      <c r="A1" t="s" s="47">
-        <v>46</v>
-      </c>
-      <c r="B1" s="48"/>
-      <c r="C1" t="s" s="47">
+      <c r="A1" t="s" s="46">
         <v>47</v>
       </c>
-      <c r="D1" s="48"/>
+      <c r="B1" s="47"/>
+      <c r="C1" t="s" s="46">
+        <v>48</v>
+      </c>
+      <c r="D1" s="47"/>
     </row>
     <row r="2" ht="23" customHeight="1">
-      <c r="A2" t="s" s="49">
-        <v>48</v>
-      </c>
-      <c r="B2" s="50">
+      <c r="A2" t="s" s="48">
+        <v>49</v>
+      </c>
+      <c r="B2" s="49">
         <v>0</v>
       </c>
-      <c r="C2" t="s" s="49">
-        <v>49</v>
-      </c>
-      <c r="D2" s="50">
+      <c r="C2" t="s" s="48">
+        <v>50</v>
+      </c>
+      <c r="D2" s="49">
         <v>0</v>
       </c>
     </row>
     <row r="3" ht="37" customHeight="1">
-      <c r="A3" t="s" s="51">
-        <v>50</v>
-      </c>
-      <c r="B3" s="52">
+      <c r="A3" t="s" s="50">
+        <v>51</v>
+      </c>
+      <c r="B3" s="51">
         <v>0</v>
       </c>
-      <c r="C3" t="s" s="51">
-        <v>51</v>
-      </c>
-      <c r="D3" t="s" s="51">
+      <c r="C3" t="s" s="50">
         <v>52</v>
       </c>
+      <c r="D3" t="s" s="50">
+        <v>53</v>
+      </c>
     </row>
     <row r="4" ht="51" customHeight="1">
-      <c r="A4" t="s" s="49">
-        <v>53</v>
-      </c>
-      <c r="B4" s="50">
+      <c r="A4" t="s" s="48">
+        <v>54</v>
+      </c>
+      <c r="B4" s="49">
         <v>0</v>
       </c>
-      <c r="C4" t="s" s="49">
-        <v>54</v>
-      </c>
-      <c r="D4" s="50">
+      <c r="C4" t="s" s="48">
+        <v>55</v>
+      </c>
+      <c r="D4" s="49">
         <f>'Compte de résultat prévisionnel'!C6</f>
-        <v>60318.995999999985</v>
+        <v>62710.395999999993</v>
       </c>
     </row>
     <row r="5" ht="23" customHeight="1">
-      <c r="A5" t="s" s="51">
-        <v>55</v>
-      </c>
-      <c r="B5" s="52">
+      <c r="A5" t="s" s="50">
+        <v>56</v>
+      </c>
+      <c r="B5" s="51">
         <v>0</v>
       </c>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
     </row>
     <row r="6" ht="23" customHeight="1">
-      <c r="A6" t="s" s="49">
-        <v>56</v>
-      </c>
-      <c r="B6" s="50">
+      <c r="A6" t="s" s="48">
+        <v>57</v>
+      </c>
+      <c r="B6" s="49">
         <v>0</v>
       </c>
-      <c r="C6" s="49"/>
-      <c r="D6" s="49"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1541,18 +1547,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.25" defaultRowHeight="21" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="12" style="53" customWidth="1"/>
-    <col min="2" max="2" width="12" style="53" customWidth="1"/>
-    <col min="3" max="256" width="12.25" style="53" customWidth="1"/>
+    <col min="1" max="1" width="12" style="52" customWidth="1"/>
+    <col min="2" max="2" width="12" style="52" customWidth="1"/>
+    <col min="3" max="256" width="12.25" style="52" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="22" customHeight="1">
-      <c r="A1" t="s" s="41">
-        <v>59</v>
-      </c>
-      <c r="B1" s="43">
+      <c r="A1" t="s" s="40">
+        <v>60</v>
+      </c>
+      <c r="B1" s="42">
         <f>'Compte de résultat prévisionnel'!C6-'Impots'!D4</f>
-        <v>34299.796799999989</v>
+        <v>34689.5968</v>
       </c>
     </row>
   </sheetData>

</xml_diff>